<commit_message>
add agreement information TC01
</commit_message>
<xml_diff>
--- a/Excel/Test_Data.xlsx
+++ b/Excel/Test_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Praful_Personal\GitProject\AMPS_Automation\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayan.thakor\Documents\PersonalWorkspace\AMPS_Automation_V2\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C470C82-BAFE-4CB7-A25D-9A536B261A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="7" r:id="rId1"/>
@@ -19,23 +20,32 @@
     <sheet name="ProjectApproval" sheetId="8" r:id="rId5"/>
     <sheet name="ProjectSettingsAndMaintence" sheetId="2" r:id="rId6"/>
     <sheet name="InterconnectionInformation" sheetId="3" r:id="rId7"/>
-    <sheet name="KeyDate" sheetId="13" r:id="rId9"/>
-    <sheet name="CountryState" sheetId="4" r:id="rId8"/>
+    <sheet name="KeyDate" sheetId="13" r:id="rId8"/>
+    <sheet name="CountryState" sheetId="4" r:id="rId9"/>
     <sheet name="ProjectAssignment" sheetId="10" r:id="rId10"/>
     <sheet name="ProjectPermit" sheetId="11" r:id="rId11"/>
     <sheet name="OperatingCompany" sheetId="12" r:id="rId12"/>
+    <sheet name="AgreementInfo" sheetId="14" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="174">
   <si>
     <t>Project Name</t>
   </si>
@@ -121,12 +131,6 @@
     <t>Project Status</t>
   </si>
   <si>
-    <t>Phoenix, City of</t>
-  </si>
-  <si>
-    <t>Prospect</t>
-  </si>
-  <si>
     <t>AddProjectALT</t>
   </si>
   <si>
@@ -199,9 +203,6 @@
     <t>AddProject2</t>
   </si>
   <si>
-    <t>https://uat.geoamps.com/dotAMPS/Login/Login.aspx</t>
-  </si>
-  <si>
     <t>ENV</t>
   </si>
   <si>
@@ -409,9 +410,6 @@
     <t>Contact Log</t>
   </si>
   <si>
-    <t>environmentALT</t>
-  </si>
-  <si>
     <t>environmentDOT</t>
   </si>
   <si>
@@ -475,9 +473,6 @@
     <t>Geo Support</t>
   </si>
   <si>
-    <t>Business Admin</t>
-  </si>
-  <si>
     <t>Appraiser</t>
   </si>
   <si>
@@ -509,13 +504,76 @@
   </si>
   <si>
     <t>https://uat.geoamps.com/Stleehead/Login/Login.aspx</t>
+  </si>
+  <si>
+    <t>AddAgreementInformationROW</t>
+  </si>
+  <si>
+    <t>AddAgreementInformationALT</t>
+  </si>
+  <si>
+    <t>AddAgreementInformationDOT</t>
+  </si>
+  <si>
+    <t>AgreementType</t>
+  </si>
+  <si>
+    <t>AgreementStatus</t>
+  </si>
+  <si>
+    <t>OperatingCompany</t>
+  </si>
+  <si>
+    <t>AgreementTerm</t>
+  </si>
+  <si>
+    <t>EffectiveDate</t>
+  </si>
+  <si>
+    <t>TermYMD</t>
+  </si>
+  <si>
+    <t>YY-MM-DD</t>
+  </si>
+  <si>
+    <t>ExpirationDate</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Long Form Renewable</t>
+  </si>
+  <si>
+    <t>Fully Executed</t>
+  </si>
+  <si>
+    <t>geoAMPS North LLC ()</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>1-0-0</t>
+  </si>
+  <si>
+    <t>Automation Comments</t>
+  </si>
+  <si>
+    <t>01/01/2023</t>
+  </si>
+  <si>
+    <t>11/01/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,15 +604,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <color rgb="FF0000FF"/>
-      <u val="single"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -600,7 +653,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -647,8 +700,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="5" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -929,14 +988,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6" activeCellId="0"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
@@ -944,7 +1003,7 @@
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -961,269 +1020,267 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="9" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="B5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="C9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="C10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="E12" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B12" r:id="rId10"/>
-    <hyperlink ref="B13" r:id="rId11"/>
-    <hyperlink ref="B14" r:id="rId12"/>
-    <hyperlink ref="B7" r:id="rId13"/>
-    <hyperlink ref="B12" r:id="rId14"/>
-    <hyperlink ref="B13" r:id="rId15"/>
-    <hyperlink ref="B6" display="https://uat.geoamps.com/Stleehead/Login/Login.aspx" r:id="rId16"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B13" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B6" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4" activeCellId="0"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="2" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1246,96 +1303,96 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1344,14 +1401,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="17" bestFit="1" customWidth="1"/>
@@ -1361,7 +1418,7 @@
     <col min="6" max="6" width="20.42578125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1381,84 +1438,84 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="C3" s="17">
         <v>12345</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C5" s="17">
         <v>45678</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1467,19 +1524,19 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1487,20 +1544,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1508,22 +1565,209 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4889DE45-9971-4E1D-895A-22B988666BDA}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -1534,48 +1778,48 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1585,70 +1829,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="B2" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="10">
         <v>3</v>
@@ -1660,15 +1904,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="B1">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4" activeCellId="0"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85547" defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="5" customWidth="1"/>
@@ -1682,7 +1926,7 @@
     <col min="10" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -1714,7 +1958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customHeight="1" ht="24" customFormat="1" s="7">
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -1737,21 +1981,21 @@
         <v>27</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" ht="27">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -1763,83 +2007,83 @@
         <v>6</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" ht="27">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" ht="30">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="I5" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1850,14 +2094,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="A9" sqref="A9" activeCellId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
@@ -1866,11 +2110,10 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="5">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -1899,120 +2142,120 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customHeight="1" ht="24" customFormat="1" s="7">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>71</v>
       </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
       <c r="I3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" t="s">
         <v>132</v>
       </c>
-      <c r="F4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" t="s">
-        <v>133</v>
-      </c>
-      <c r="H4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H5" t="s">
-        <v>136</v>
-      </c>
       <c r="I5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2021,19 +2264,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="41.2852" defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="41.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="41.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2041,7 +2284,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customHeight="1" ht="24" customFormat="1" s="2">
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2049,18 +2292,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
   </sheetData>
@@ -2069,14 +2312,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85547" defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
@@ -2086,7 +2329,7 @@
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -2103,7 +2346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customHeight="1" ht="24" customFormat="1" s="2">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -2114,15 +2357,15 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -2137,9 +2380,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -2154,9 +2397,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -2177,154 +2420,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -2333,7 +2436,7 @@
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -2350,26 +2453,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" s="12">
         <v>44805</v>
@@ -2384,9 +2487,9 @@
         <v>44864</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B4" s="12">
         <v>44805</v>
@@ -2404,4 +2507,143 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agreement Testcase 02-03-04 added
</commit_message>
<xml_diff>
--- a/Excel/Test_Data.xlsx
+++ b/Excel/Test_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nayan.thakor\Documents\PersonalWorkspace\AMPS_Automation_V2\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C470C82-BAFE-4CB7-A25D-9A536B261A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AA7966-F343-4ECB-86B1-B3578AD33289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="847" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="7" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="ProjectPermit" sheetId="11" r:id="rId11"/>
     <sheet name="OperatingCompany" sheetId="12" r:id="rId12"/>
     <sheet name="AgreementInfo" sheetId="14" r:id="rId13"/>
+    <sheet name="PayeeInfo" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="177">
   <si>
     <t>Project Name</t>
   </si>
@@ -512,9 +513,6 @@
     <t>AddAgreementInformationALT</t>
   </si>
   <si>
-    <t>AddAgreementInformationDOT</t>
-  </si>
-  <si>
     <t>AgreementType</t>
   </si>
   <si>
@@ -567,6 +565,18 @@
   </si>
   <si>
     <t>11/01/2024</t>
+  </si>
+  <si>
+    <t>AddPayeeInformationALT</t>
+  </si>
+  <si>
+    <t>LandownerName</t>
+  </si>
+  <si>
+    <t>Parcel #: test1, Grantor Name: , County PID:</t>
+  </si>
+  <si>
+    <t>AvailableTract</t>
   </si>
 </sst>
 </file>
@@ -1567,10 +1577,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4889DE45-9971-4E1D-895A-22B988666BDA}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1616,7 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
         <v>13</v>
@@ -1623,31 +1633,31 @@
         <v>12</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>161</v>
-      </c>
       <c r="H2" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="21" t="s">
         <v>164</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1655,100 +1665,121 @@
         <v>154</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>167</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>168</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" t="s">
         <v>169</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>172</v>
-      </c>
-      <c r="G3" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>173</v>
       </c>
       <c r="I3">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" t="s">
         <v>166</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>167</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>168</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="G4" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>172</v>
-      </c>
-      <c r="G4" t="s">
-        <v>170</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>173</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="C5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F5" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="G5" t="s">
         <v>170</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="I5">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76DE2ED-E37E-42FD-8666-BDDBB73E2639}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>